<commit_message>
all c14 plots basically done
</commit_message>
<xml_diff>
--- a/data/Sites.xlsx
+++ b/data/Sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cylerconrad/Dropbox/Radiocarbon_Antiquity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/14C_Antiquity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7651945A-594A-6040-B218-64CC3CCAB367}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{FAD6BABC-439A-0148-B93B-3F443DE2DE67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3320" yWindow="2620" windowWidth="25200" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Cyler - Personal View" guid="{02E70EBB-E010-4DDD-AC0E-6E0B7A77DFC9}" mergeInterval="0" personalView="1" xWindow="510" windowWidth="856" windowHeight="728" activeSheetId="1"/>
+    <customWorkbookView name="Joyce White - Personal View" guid="{FD9AD598-8900-4182-B3BB-55F6A6A0EDD5}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="BC-WS - Personal View" guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}" mergeInterval="0" personalView="1" xWindow="52" yWindow="49" windowWidth="821" windowHeight="1001" activeSheetId="1"/>
+    <customWorkbookView name="BC volunteer - Personal View" guid="{8F6E6FA8-D877-4F31-9037-ECEBE3B3DF3D}" mergeInterval="0" personalView="1" xWindow="858" windowWidth="818" windowHeight="1004" activeSheetId="1"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{B101061E-A013-C44B-BA56-887481C8E808}" mergeInterval="0" personalView="1" xWindow="166" yWindow="131" windowWidth="1260" windowHeight="558" activeSheetId="1"/>
-    <customWorkbookView name="BC volunteer - Personal View" guid="{8F6E6FA8-D877-4F31-9037-ECEBE3B3DF3D}" mergeInterval="0" personalView="1" xWindow="858" windowWidth="818" windowHeight="1004" activeSheetId="1"/>
-    <customWorkbookView name="BC-WS - Personal View" guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}" mergeInterval="0" personalView="1" xWindow="52" yWindow="49" windowWidth="821" windowHeight="1001" activeSheetId="1"/>
-    <customWorkbookView name="Joyce White - Personal View" guid="{FD9AD598-8900-4182-B3BB-55F6A6A0EDD5}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="Cyler - Personal View" guid="{02E70EBB-E010-4DDD-AC0E-6E0B7A77DFC9}" mergeInterval="0" personalView="1" xWindow="510" windowWidth="856" windowHeight="728" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -68,13 +68,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,13 +103,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -127,13 +134,49 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8A8AF59B-17FA-9444-BC10-0FCB0E434C04}" diskRevisions="1" revisionId="672" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1612BADB-37B3-F941-8108-3E932EC2C2B7}" diskRevisions="1" revisionId="674" version="3">
   <header guid="{8A8AF59B-17FA-9444-BC10-0FCB0E434C04}" dateTime="2020-12-17T11:45:01" maxSheetId="2" userName="Microsoft Office User" r:id="rId53" minRId="515" maxRId="672">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{1612BADB-37B3-F941-8108-3E932EC2C2B7}" dateTime="2020-12-17T18:49:40" maxSheetId="2" userName="Microsoft Office User" r:id="rId54" minRId="673" maxRId="674">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" xfDxf="1" sqref="B3" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="673" sId="1">
+    <oc r="B3">
+      <v>19.516666669999999</v>
+    </oc>
+    <nc r="B3">
+      <v>19.545241999999998</v>
+    </nc>
+  </rcc>
+  <rcc rId="674" sId="1">
+    <oc r="C3">
+      <v>98.516666670000006</v>
+    </oc>
+    <nc r="C3">
+      <v>98.194604999999996</v>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17005,7 +17048,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17026,15 +17069,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:177" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:177" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>19.516666669999999</v>
+      <c r="B2" s="4">
+        <v>19.545241999999998</v>
       </c>
       <c r="C2" s="2">
-        <v>98.516666670000006</v>
+        <v>98.194604999999996</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -17258,29 +17301,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B101061E-A013-C44B-BA56-887481C8E808}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    <customSheetView guid="{02E70EBB-E010-4DDD-AC0E-6E0B7A77DFC9}" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{FD9AD598-8900-4182-B3BB-55F6A6A0EDD5}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}">
+      <selection activeCell="A13" sqref="A13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{8F6E6FA8-D877-4F31-9037-ECEBE3B3DF3D}" topLeftCell="A106">
       <selection activeCell="E124" sqref="E124"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}">
-      <selection activeCell="A13" sqref="A13"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{FD9AD598-8900-4182-B3BB-55F6A6A0EDD5}">
+    <customSheetView guid="{B101061E-A013-C44B-BA56-887481C8E808}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{02E70EBB-E010-4DDD-AC0E-6E0B7A77DFC9}" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
     </customSheetView>
@@ -17303,21 +17346,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100702D1BEEAE0DE84A869658185257158C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8a2b66bdc77e042f083b234d6bcebfef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="893aec1e-09f0-4637-b3f9-0343a3d770de" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aa2b905494d554e246f03a23035eea03" ns2:_="">
     <xsd:import namespace="893aec1e-09f0-4637-b3f9-0343a3d770de"/>
@@ -17449,10 +17477,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{016F23F0-4E73-4288-B2DA-1D184FB023BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BB30F1-9342-4650-AC32-026F56B09C01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="893aec1e-09f0-4637-b3f9-0343a3d770de"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17474,19 +17527,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BB30F1-9342-4650-AC32-026F56B09C01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{016F23F0-4E73-4288-B2DA-1D184FB023BA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="893aec1e-09f0-4637-b3f9-0343a3d770de"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change spelling of Tham Pha Can on map
</commit_message>
<xml_diff>
--- a/data/Sites.xlsx
+++ b/data/Sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/14C_Antiquity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{FAD6BABC-439A-0148-B93B-3F443DE2DE67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{630BEC03-2A89-5943-92C4-519265C75BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3320" yWindow="2620" windowWidth="25200" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,11 +23,11 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{B101061E-A013-C44B-BA56-887481C8E808}" mergeInterval="0" personalView="1" xWindow="166" yWindow="131" windowWidth="1260" windowHeight="558" activeSheetId="1"/>
+    <customWorkbookView name="BC volunteer - Personal View" guid="{8F6E6FA8-D877-4F31-9037-ECEBE3B3DF3D}" mergeInterval="0" personalView="1" xWindow="858" windowWidth="818" windowHeight="1004" activeSheetId="1"/>
+    <customWorkbookView name="BC-WS - Personal View" guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}" mergeInterval="0" personalView="1" xWindow="52" yWindow="49" windowWidth="821" windowHeight="1001" activeSheetId="1"/>
+    <customWorkbookView name="Joyce White - Personal View" guid="{FD9AD598-8900-4182-B3BB-55F6A6A0EDD5}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Cyler - Personal View" guid="{02E70EBB-E010-4DDD-AC0E-6E0B7A77DFC9}" mergeInterval="0" personalView="1" xWindow="510" windowWidth="856" windowHeight="728" activeSheetId="1"/>
-    <customWorkbookView name="Joyce White - Personal View" guid="{FD9AD598-8900-4182-B3BB-55F6A6A0EDD5}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="BC-WS - Personal View" guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}" mergeInterval="0" personalView="1" xWindow="52" yWindow="49" windowWidth="821" windowHeight="1001" activeSheetId="1"/>
-    <customWorkbookView name="BC volunteer - Personal View" guid="{8F6E6FA8-D877-4F31-9037-ECEBE3B3DF3D}" mergeInterval="0" personalView="1" xWindow="858" windowWidth="818" windowHeight="1004" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{B101061E-A013-C44B-BA56-887481C8E808}" mergeInterval="0" personalView="1" xWindow="166" yWindow="131" windowWidth="1260" windowHeight="558" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,13 +55,13 @@
     <t>Spirit Cave</t>
   </si>
   <si>
-    <t xml:space="preserve">Tham Phaa Can </t>
-  </si>
-  <si>
     <t>Banyan Valley Cave</t>
   </si>
   <si>
     <t>Tham Lod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tham Pha Can </t>
   </si>
 </sst>
 </file>
@@ -134,13 +134,18 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1612BADB-37B3-F941-8108-3E932EC2C2B7}" diskRevisions="1" revisionId="674" version="3">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{65C0BD08-4220-7045-80B9-40BCF360A4DF}" diskRevisions="1" revisionId="675" version="4">
   <header guid="{8A8AF59B-17FA-9444-BC10-0FCB0E434C04}" dateTime="2020-12-17T11:45:01" maxSheetId="2" userName="Microsoft Office User" r:id="rId53" minRId="515" maxRId="672">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
   <header guid="{1612BADB-37B3-F941-8108-3E932EC2C2B7}" dateTime="2020-12-17T18:49:40" maxSheetId="2" userName="Microsoft Office User" r:id="rId54" minRId="673" maxRId="674">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{65C0BD08-4220-7045-80B9-40BCF360A4DF}" dateTime="2020-12-21T13:02:42" maxSheetId="2" userName="Microsoft Office User" r:id="rId55" minRId="675">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -174,6 +179,23 @@
     </oc>
     <nc r="C3">
       <v>98.194604999999996</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="675" sId="1">
+    <oc r="A6" t="inlineStr">
+      <is>
+        <t xml:space="preserve">Tham Phaa Can </t>
+      </is>
+    </oc>
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t xml:space="preserve">Tham Pha Can </t>
+      </is>
     </nc>
   </rcc>
 </revisions>
@@ -17048,7 +17070,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17256,7 +17278,7 @@
     </row>
     <row r="3" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>19.630880999999999</v>
@@ -17279,7 +17301,7 @@
     </row>
     <row r="5" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3">
         <v>19.231849</v>
@@ -17290,7 +17312,7 @@
     </row>
     <row r="6" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>19.567578361359001</v>
@@ -17301,29 +17323,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{02E70EBB-E010-4DDD-AC0E-6E0B7A77DFC9}" topLeftCell="B1">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+    <customSheetView guid="{B101061E-A013-C44B-BA56-887481C8E808}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{8F6E6FA8-D877-4F31-9037-ECEBE3B3DF3D}" topLeftCell="A106">
+      <selection activeCell="E124" sqref="E124"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+    </customSheetView>
+    <customSheetView guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}">
+      <selection activeCell="A13" sqref="A13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{FD9AD598-8900-4182-B3BB-55F6A6A0EDD5}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{77C47E83-598B-43A8-BE56-CB5A29D076B1}">
-      <selection activeCell="A13" sqref="A13"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{8F6E6FA8-D877-4F31-9037-ECEBE3B3DF3D}" topLeftCell="A106">
-      <selection activeCell="E124" sqref="E124"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{B101061E-A013-C44B-BA56-887481C8E808}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    <customSheetView guid="{02E70EBB-E010-4DDD-AC0E-6E0B7A77DFC9}" topLeftCell="B1">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
     </customSheetView>
@@ -17346,6 +17368,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100702D1BEEAE0DE84A869658185257158C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8a2b66bdc77e042f083b234d6bcebfef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="893aec1e-09f0-4637-b3f9-0343a3d770de" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aa2b905494d554e246f03a23035eea03" ns2:_="">
     <xsd:import namespace="893aec1e-09f0-4637-b3f9-0343a3d770de"/>
@@ -17477,35 +17514,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BB30F1-9342-4650-AC32-026F56B09C01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{016F23F0-4E73-4288-B2DA-1D184FB023BA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="893aec1e-09f0-4637-b3f9-0343a3d770de"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17527,9 +17539,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{016F23F0-4E73-4288-B2DA-1D184FB023BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BB30F1-9342-4650-AC32-026F56B09C01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="893aec1e-09f0-4637-b3f9-0343a3d770de"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>